<commit_message>
updated calibration targets to exclude buses
</commit_message>
<xml_diff>
--- a/abm2p/Final CVM Overall Calibration Targets.xlsx
+++ b/abm2p/Final CVM Overall Calibration Targets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iya\Dev\CVM\Data_CVM\abm2p\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676BC471-2390-4768-96A7-191F2D7FFEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96674796-A875-4619-86C0-F8C5F8DBE4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="21600" windowHeight="13869" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,7 +144,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,6 +190,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -204,10 +215,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -231,9 +243,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -512,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -586,34 +602,34 @@
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="9">
         <v>935</v>
       </c>
-      <c r="C3">
-        <v>2386.8212149999999</v>
-      </c>
-      <c r="D3">
-        <v>12155.782078</v>
-      </c>
-      <c r="E3">
+      <c r="C3" s="9">
+        <v>2386.8200000000002</v>
+      </c>
+      <c r="D3" s="9">
+        <v>12155.78</v>
+      </c>
+      <c r="E3" s="9">
         <v>94294.62</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="9">
         <v>75846.320000000007</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="11">
         <f t="shared" ref="G3:G14" si="0">C3/B3</f>
-        <v>2.5527499625668448</v>
-      </c>
-      <c r="H3">
+        <v>2.5527486631016045</v>
+      </c>
+      <c r="H3" s="11">
         <f t="shared" ref="H3:H14" si="1">D3/C3</f>
-        <v>5.0928749927337984</v>
-      </c>
-      <c r="I3">
+        <v>5.0928767146244791</v>
+      </c>
+      <c r="I3" s="11">
         <f t="shared" ref="I3:I14" si="2">E3/D3</f>
-        <v>7.7571824992369685</v>
-      </c>
-      <c r="J3">
+        <v>7.7571838253077949</v>
+      </c>
+      <c r="J3" s="11">
         <f t="shared" ref="J3:J14" si="3">1-(F3/E3)</f>
         <v>0.19564530829012294</v>
       </c>
@@ -622,34 +638,34 @@
       <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="9">
         <v>38763</v>
       </c>
-      <c r="C4">
-        <v>22801.712597000002</v>
-      </c>
-      <c r="D4">
-        <v>120978.73553999999</v>
-      </c>
-      <c r="E4">
+      <c r="C4" s="9">
+        <v>22801.71</v>
+      </c>
+      <c r="D4" s="9">
+        <v>120978.74</v>
+      </c>
+      <c r="E4" s="9">
         <v>1455627.51</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="9">
         <v>1252495.6299999999</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="11">
         <f t="shared" si="0"/>
-        <v>0.58823394982328514</v>
-      </c>
-      <c r="H4">
+        <v>0.58823388282640665</v>
+      </c>
+      <c r="H4" s="11">
         <f t="shared" si="1"/>
-        <v>5.3056863612918725</v>
-      </c>
-      <c r="I4">
+        <v>5.3056871611822096</v>
+      </c>
+      <c r="I4" s="11">
         <f t="shared" si="2"/>
-        <v>12.032093933720413</v>
-      </c>
-      <c r="J4">
+        <v>12.032093490145458</v>
+      </c>
+      <c r="J4" s="11">
         <f t="shared" si="3"/>
         <v>0.13954935490330223</v>
       </c>
@@ -658,34 +674,34 @@
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="9">
         <v>192374</v>
       </c>
-      <c r="C5">
-        <v>5409.1769340000001</v>
-      </c>
-      <c r="D5">
-        <v>21123.987943</v>
-      </c>
-      <c r="E5">
+      <c r="C5" s="9">
+        <v>5409.18</v>
+      </c>
+      <c r="D5" s="9">
+        <v>21123.99</v>
+      </c>
+      <c r="E5" s="9">
         <v>94476.61</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="9">
         <v>53948.85</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="11">
         <f t="shared" si="0"/>
-        <v>2.8118024961793175E-2</v>
-      </c>
-      <c r="H5">
+        <v>2.8118040899497855E-2</v>
+      </c>
+      <c r="H5" s="11">
         <f t="shared" si="1"/>
-        <v>3.9052129743108899</v>
-      </c>
-      <c r="I5">
+        <v>3.9052111410601977</v>
+      </c>
+      <c r="I5" s="11">
         <f t="shared" si="2"/>
-        <v>4.4724798297997213</v>
-      </c>
-      <c r="J5">
+        <v>4.4724793942810992</v>
+      </c>
+      <c r="J5" s="11">
         <f t="shared" si="3"/>
         <v>0.42897136127132418</v>
       </c>
@@ -694,34 +710,34 @@
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="9">
         <v>176056</v>
       </c>
-      <c r="C6">
-        <v>18768.581199</v>
-      </c>
-      <c r="D6">
-        <v>94282.137992999997</v>
-      </c>
-      <c r="E6">
+      <c r="C6" s="9">
+        <v>18768.580000000002</v>
+      </c>
+      <c r="D6" s="9">
+        <v>94282.14</v>
+      </c>
+      <c r="E6" s="9">
         <v>662266.36</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="9">
         <v>381875.91</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="11">
         <f t="shared" si="0"/>
-        <v>0.10660574589335212</v>
-      </c>
-      <c r="H6">
+        <v>0.10660573908301905</v>
+      </c>
+      <c r="H6" s="11">
         <f t="shared" si="1"/>
-        <v>5.023402514731556</v>
-      </c>
-      <c r="I6">
+        <v>5.0234029425774347</v>
+      </c>
+      <c r="I6" s="11">
         <f t="shared" si="2"/>
-        <v>7.0243035860002472</v>
-      </c>
-      <c r="J6">
+        <v>7.0243034364726977</v>
+      </c>
+      <c r="J6" s="11">
         <f t="shared" si="3"/>
         <v>0.423380178935859</v>
       </c>
@@ -730,34 +746,34 @@
       <c r="A7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="9">
         <v>219675</v>
       </c>
-      <c r="C7">
-        <v>13948.570087</v>
-      </c>
-      <c r="D7">
-        <v>79692.935931</v>
-      </c>
-      <c r="E7">
+      <c r="C7" s="9">
+        <v>13948.57</v>
+      </c>
+      <c r="D7" s="9">
+        <v>79692.94</v>
+      </c>
+      <c r="E7" s="9">
         <v>1054351.58</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="9">
         <v>412153.19</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="11">
         <f t="shared" si="0"/>
-        <v>6.3496392793900083E-2</v>
-      </c>
-      <c r="H7">
+        <v>6.3496392397860479E-2</v>
+      </c>
+      <c r="H7" s="11">
         <f t="shared" si="1"/>
-        <v>5.7133408968761197</v>
-      </c>
-      <c r="I7">
+        <v>5.7133412242258528</v>
+      </c>
+      <c r="I7" s="11">
         <f t="shared" si="2"/>
-        <v>13.230176146514193</v>
-      </c>
-      <c r="J7">
+        <v>13.230175471001573</v>
+      </c>
+      <c r="J7" s="11">
         <f t="shared" si="3"/>
         <v>0.60909321158317997</v>
       </c>
@@ -766,34 +782,34 @@
       <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="9">
         <v>201506</v>
       </c>
-      <c r="C8">
-        <v>42326.071739999999</v>
-      </c>
-      <c r="D8">
-        <v>200942.19612099999</v>
-      </c>
-      <c r="E8">
+      <c r="C8" s="9">
+        <v>42326.07</v>
+      </c>
+      <c r="D8" s="9">
+        <v>200942.2</v>
+      </c>
+      <c r="E8" s="9">
         <v>1996970.71</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="9">
         <v>1007088.57</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="11">
         <f t="shared" si="0"/>
-        <v>0.210048692048872</v>
-      </c>
-      <c r="H8">
+        <v>0.21004868341389338</v>
+      </c>
+      <c r="H8" s="11">
         <f t="shared" si="1"/>
-        <v>4.7474804029853015</v>
-      </c>
-      <c r="I8">
+        <v>4.7474806897970927</v>
+      </c>
+      <c r="I8" s="11">
         <f t="shared" si="2"/>
-        <v>9.9380356567691628</v>
-      </c>
-      <c r="J8">
+        <v>9.938035464924738</v>
+      </c>
+      <c r="J8" s="11">
         <f t="shared" si="3"/>
         <v>0.49569186720820757</v>
       </c>
@@ -802,106 +818,106 @@
       <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="9">
         <v>187372</v>
       </c>
-      <c r="C9">
-        <v>12798.121198999999</v>
-      </c>
-      <c r="D9">
-        <v>102064.118758</v>
-      </c>
-      <c r="E9">
-        <v>753000.36</v>
-      </c>
-      <c r="F9">
-        <v>367360.34</v>
-      </c>
-      <c r="G9">
+      <c r="C9" s="9">
+        <v>11813.85</v>
+      </c>
+      <c r="D9" s="9">
+        <v>96814.66</v>
+      </c>
+      <c r="E9" s="9">
+        <v>700589.36</v>
+      </c>
+      <c r="F9" s="9">
+        <v>314949.34000000003</v>
+      </c>
+      <c r="G9" s="11">
         <f t="shared" si="0"/>
-        <v>6.8303274763571925E-2</v>
-      </c>
-      <c r="H9">
+        <v>6.3050242298742606E-2</v>
+      </c>
+      <c r="H9" s="11">
         <f t="shared" si="1"/>
-        <v>7.9749298487636553</v>
-      </c>
-      <c r="I9">
+        <v>8.1950134799409167</v>
+      </c>
+      <c r="I9" s="11">
         <f t="shared" si="2"/>
-        <v>7.3777187239073498</v>
-      </c>
-      <c r="J9">
+        <v>7.2363974629462104</v>
+      </c>
+      <c r="J9" s="11">
         <f t="shared" si="3"/>
-        <v>0.51213789592344949</v>
+        <v>0.55045086611078409</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="9">
         <v>52170</v>
       </c>
-      <c r="C10">
-        <v>57081.146076999998</v>
-      </c>
-      <c r="D10">
-        <v>262026.912698</v>
-      </c>
-      <c r="E10">
-        <v>2000252.9</v>
-      </c>
-      <c r="F10">
-        <v>474896.71</v>
-      </c>
-      <c r="G10">
+      <c r="C10" s="9">
+        <v>55873.74</v>
+      </c>
+      <c r="D10" s="9">
+        <v>259008.39</v>
+      </c>
+      <c r="E10" s="9">
+        <v>1955834.77</v>
+      </c>
+      <c r="F10" s="9">
+        <v>430478.58</v>
+      </c>
+      <c r="G10" s="11">
         <f t="shared" si="0"/>
-        <v>1.094137360111175</v>
-      </c>
-      <c r="H10">
+        <v>1.0709936745255895</v>
+      </c>
+      <c r="H10" s="11">
         <f t="shared" si="1"/>
-        <v>4.5904283762021354</v>
-      </c>
-      <c r="I10">
+        <v>4.6356014471198819</v>
+      </c>
+      <c r="I10" s="11">
         <f t="shared" si="2"/>
-        <v>7.6337689110026581</v>
-      </c>
-      <c r="J10">
+        <v>7.55124098489628</v>
+      </c>
+      <c r="J10" s="11">
         <f t="shared" si="3"/>
-        <v>0.76258166654826498</v>
+        <v>0.77990033380989543</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="9">
         <v>4829</v>
       </c>
-      <c r="C11">
-        <v>84795.471911000001</v>
-      </c>
-      <c r="D11">
-        <v>538669.75641100004</v>
-      </c>
-      <c r="E11">
+      <c r="C11" s="9">
+        <v>84795.47</v>
+      </c>
+      <c r="D11" s="9">
+        <v>538669.76</v>
+      </c>
+      <c r="E11" s="9">
         <v>2830538.79</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="9">
         <v>1205466.6100000001</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="11">
         <f t="shared" si="0"/>
-        <v>17.559633860219506</v>
-      </c>
-      <c r="H11">
+        <v>17.559633464485401</v>
+      </c>
+      <c r="H11" s="11">
         <f t="shared" si="1"/>
-        <v>6.3525769038278295</v>
-      </c>
-      <c r="I11">
+        <v>6.3525770893185687</v>
+      </c>
+      <c r="I11" s="11">
         <f t="shared" si="2"/>
-        <v>5.2546829598510545</v>
-      </c>
-      <c r="J11">
+        <v>5.2546829248406297</v>
+      </c>
+      <c r="J11" s="11">
         <f t="shared" si="3"/>
         <v>0.57412114815073778</v>
       </c>
@@ -910,70 +926,70 @@
       <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="9">
         <v>304943</v>
       </c>
-      <c r="C12">
-        <v>51360.682481999997</v>
-      </c>
-      <c r="D12">
-        <v>416510.497271</v>
-      </c>
-      <c r="E12">
-        <v>3226709.41</v>
-      </c>
-      <c r="F12">
-        <v>1347647.49</v>
-      </c>
-      <c r="G12">
+      <c r="C12" s="9">
+        <v>47738.45</v>
+      </c>
+      <c r="D12" s="9">
+        <v>400210.47</v>
+      </c>
+      <c r="E12" s="9">
+        <v>3162765.3</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1283703.3799999999</v>
+      </c>
+      <c r="G12" s="11">
         <f t="shared" si="0"/>
-        <v>0.16842715681947118</v>
-      </c>
-      <c r="H12">
+        <v>0.15654876485113611</v>
+      </c>
+      <c r="H12" s="11">
         <f t="shared" si="1"/>
-        <v>8.1095203011948183</v>
-      </c>
-      <c r="I12">
+        <v>8.3833989163871045</v>
+      </c>
+      <c r="I12" s="11">
         <f t="shared" si="2"/>
-        <v>7.7470062126683006</v>
-      </c>
-      <c r="J12">
+        <v>7.9027550178784676</v>
+      </c>
+      <c r="J12" s="11">
         <f t="shared" si="3"/>
-        <v>0.58234618654426651</v>
+        <v>0.5941199367528156</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="9">
         <v>83282</v>
       </c>
-      <c r="C13">
-        <v>9532.9175510000005</v>
-      </c>
-      <c r="D13">
-        <v>38822.653095000001</v>
-      </c>
-      <c r="E13">
+      <c r="C13" s="9">
+        <v>9532.92</v>
+      </c>
+      <c r="D13" s="9">
+        <v>38822.65</v>
+      </c>
+      <c r="E13" s="9">
         <v>254478</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="9">
         <v>33967.440000000002</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="11">
         <f t="shared" si="0"/>
-        <v>0.11446552137316587</v>
-      </c>
-      <c r="H13">
+        <v>0.11446555077928004</v>
+      </c>
+      <c r="H13" s="11">
         <f t="shared" si="1"/>
-        <v>4.0724838841103281</v>
-      </c>
-      <c r="I13">
+        <v>4.0724825132278459</v>
+      </c>
+      <c r="I13" s="11">
         <f t="shared" si="2"/>
-        <v>6.5548843191444437</v>
-      </c>
-      <c r="J13">
+        <v>6.5548848417096721</v>
+      </c>
+      <c r="J13" s="11">
         <f t="shared" si="3"/>
         <v>0.86652111380944519</v>
       </c>
@@ -982,41 +998,41 @@
       <c r="A14" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="10">
         <f t="shared" ref="B14:F14" si="4">SUM(B3:B13)</f>
         <v>1461905</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="10">
         <f t="shared" si="4"/>
-        <v>321209.27299200004</v>
-      </c>
-      <c r="D14" s="7">
+        <v>315395.36</v>
+      </c>
+      <c r="D14" s="10">
         <f t="shared" si="4"/>
-        <v>1887269.7138389996</v>
-      </c>
-      <c r="E14" s="7">
+        <v>1862701.72</v>
+      </c>
+      <c r="E14" s="10">
         <f t="shared" si="4"/>
-        <v>14422966.850000001</v>
-      </c>
-      <c r="F14" s="7">
+        <v>14262193.610000003</v>
+      </c>
+      <c r="F14" s="10">
         <f t="shared" si="4"/>
-        <v>6612747.0600000005</v>
-      </c>
-      <c r="G14" s="7">
+        <v>6451973.8200000003</v>
+      </c>
+      <c r="G14" s="12">
         <f t="shared" si="0"/>
-        <v>0.21971966235288889</v>
-      </c>
-      <c r="H14" s="7">
+        <v>0.21574271926014343</v>
+      </c>
+      <c r="H14" s="12">
         <f t="shared" si="1"/>
-        <v>5.8755144154446732</v>
-      </c>
-      <c r="I14" s="7">
+        <v>5.9059262000557018</v>
+      </c>
+      <c r="I14" s="12">
         <f t="shared" si="2"/>
-        <v>7.6422393387861067</v>
-      </c>
-      <c r="J14" s="7">
+        <v>7.6567243466119761</v>
+      </c>
+      <c r="J14" s="12">
         <f t="shared" si="3"/>
-        <v>0.54151270478722624</v>
+        <v>0.54761700784399892</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
@@ -1065,7 +1081,7 @@
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A20" s="9" t="s">
+      <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" t="s">
@@ -1110,34 +1126,34 @@
       <c r="A22" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="9">
         <v>219675</v>
       </c>
-      <c r="C22">
-        <v>13948.570087</v>
-      </c>
-      <c r="D22">
-        <v>79692.935931</v>
-      </c>
-      <c r="E22">
+      <c r="C22" s="9">
+        <v>13948.57</v>
+      </c>
+      <c r="D22" s="9">
+        <v>79692.94</v>
+      </c>
+      <c r="E22" s="9">
         <v>1054351.58</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="9">
         <v>412153.19</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="11">
         <f t="shared" ref="G22:G23" si="5">C22/B22</f>
-        <v>6.3496392793900083E-2</v>
-      </c>
-      <c r="H22">
+        <v>6.3496392397860479E-2</v>
+      </c>
+      <c r="H22" s="11">
         <f t="shared" ref="H22:H23" si="6">D22/C22</f>
-        <v>5.7133408968761197</v>
-      </c>
-      <c r="I22">
+        <v>5.7133412242258528</v>
+      </c>
+      <c r="I22" s="11">
         <f t="shared" ref="I22:I23" si="7">E22/D22</f>
-        <v>13.230176146514193</v>
-      </c>
-      <c r="J22">
+        <v>13.230175471001573</v>
+      </c>
+      <c r="J22" s="11">
         <f t="shared" ref="J22:J23" si="8">1-(F22/E22)</f>
         <v>0.60909321158317997</v>
       </c>
@@ -1146,34 +1162,34 @@
       <c r="A23" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="9">
         <v>176056</v>
       </c>
-      <c r="C23">
-        <v>18768.581199</v>
-      </c>
-      <c r="D23">
-        <v>94282.137992999997</v>
-      </c>
-      <c r="E23">
+      <c r="C23" s="9">
+        <v>18768.580000000002</v>
+      </c>
+      <c r="D23" s="9">
+        <v>94282.14</v>
+      </c>
+      <c r="E23" s="9">
         <v>662266.36</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="9">
         <v>381875.91</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="11">
         <f t="shared" si="5"/>
-        <v>0.10660574589335212</v>
-      </c>
-      <c r="H23">
+        <v>0.10660573908301905</v>
+      </c>
+      <c r="H23" s="11">
         <f t="shared" si="6"/>
-        <v>5.023402514731556</v>
-      </c>
-      <c r="I23">
+        <v>5.0234029425774347</v>
+      </c>
+      <c r="I23" s="11">
         <f t="shared" si="7"/>
-        <v>7.0243035860002472</v>
-      </c>
-      <c r="J23">
+        <v>7.0243034364726977</v>
+      </c>
+      <c r="J23" s="11">
         <f t="shared" si="8"/>
         <v>0.423380178935859</v>
       </c>
@@ -1241,24 +1257,166 @@
       <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="D31" s="1"/>
-      <c r="E31" s="3"/>
+      <c r="B31" s="1">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="3">
+        <v>75846.320000000007</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="D32" s="1"/>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1">
+        <v>2</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1252495.6299999999</v>
+      </c>
       <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.4">
-      <c r="D33" s="1"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B33" s="1">
+        <v>2</v>
+      </c>
+      <c r="C33" s="1">
+        <v>3</v>
+      </c>
+      <c r="D33" s="3">
+        <v>53948.85</v>
+      </c>
       <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.4">
-      <c r="D34" s="1"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B34" s="1">
+        <v>3</v>
+      </c>
+      <c r="C34" s="1">
+        <v>4</v>
+      </c>
+      <c r="D34" s="3">
+        <v>381875.91</v>
+      </c>
       <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.4">
-      <c r="D35" s="1"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B35" s="1">
+        <v>4</v>
+      </c>
+      <c r="C35" s="1">
+        <v>5</v>
+      </c>
+      <c r="D35" s="3">
+        <v>412153.19</v>
+      </c>
       <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B36" s="1">
+        <v>5</v>
+      </c>
+      <c r="C36" s="1">
+        <v>6</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1007088.57</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B37" s="1">
+        <v>6</v>
+      </c>
+      <c r="C37" s="1">
+        <v>7</v>
+      </c>
+      <c r="D37" s="3">
+        <v>314949.34000000003</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B38" s="1">
+        <v>7</v>
+      </c>
+      <c r="C38" s="1">
+        <v>8</v>
+      </c>
+      <c r="D38" s="3">
+        <v>430478.58</v>
+      </c>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B39" s="1">
+        <v>8</v>
+      </c>
+      <c r="C39" s="1">
+        <v>9</v>
+      </c>
+      <c r="D39" s="3">
+        <v>1205466.6100000001</v>
+      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B40" s="1">
+        <v>9</v>
+      </c>
+      <c r="C40" s="1">
+        <v>10</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1283703.3799999999</v>
+      </c>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B41" s="1">
+        <v>10</v>
+      </c>
+      <c r="C41" s="1">
+        <v>11</v>
+      </c>
+      <c r="D41" s="3">
+        <v>33967.440000000002</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>